<commit_message>
FCU ready for testing
</commit_message>
<xml_diff>
--- a/Forwarding_ControlUnit/Comparisons.xlsx
+++ b/Forwarding_ControlUnit/Comparisons.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA788949-DCA8-4840-B2D2-A2E67D8F422C}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6005C38F-260F-4BC7-881C-18CB2B2348F0}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="113">
   <si>
     <t>Gli OPCODE di interesse sono REG, IMM, LW, SW e JMP</t>
   </si>
@@ -368,6 +368,9 @@
   </si>
   <si>
     <t>ID/EX.Op = IS &amp;&amp; IF/ID.Op = JMP &amp;&amp; ID/EX11..15 = IF/ID6..10</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -861,8 +864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B77" workbookViewId="0">
-      <selection activeCell="G78" sqref="G78"/>
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="C90" sqref="C90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1418,7 +1421,9 @@
         <v>86</v>
       </c>
       <c r="B72" s="17"/>
-      <c r="C72" s="17"/>
+      <c r="C72" s="17" t="s">
+        <v>112</v>
+      </c>
       <c r="D72" s="20" t="s">
         <v>87</v>
       </c>
@@ -1567,7 +1572,9 @@
         <v>94</v>
       </c>
       <c r="B77" s="17"/>
-      <c r="C77" s="17"/>
+      <c r="C77" s="17" t="s">
+        <v>112</v>
+      </c>
       <c r="D77" s="17"/>
       <c r="E77" s="17"/>
       <c r="F77" s="17"/>
@@ -1650,7 +1657,9 @@
         <v>96</v>
       </c>
       <c r="B80" s="17"/>
-      <c r="C80" s="17"/>
+      <c r="C80" s="17" t="s">
+        <v>112</v>
+      </c>
       <c r="D80" s="17"/>
       <c r="E80" s="17"/>
       <c r="F80" s="17"/>
@@ -1924,7 +1933,9 @@
         <v>104</v>
       </c>
       <c r="B90" s="17"/>
-      <c r="C90" s="17"/>
+      <c r="C90" s="17" t="s">
+        <v>112</v>
+      </c>
       <c r="D90" s="17"/>
       <c r="E90" s="17"/>
       <c r="F90" s="17"/>

</xml_diff>